<commit_message>
minor edits to component list
</commit_message>
<xml_diff>
--- a/source/implementation/data/components.xlsx
+++ b/source/implementation/data/components.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21721"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="24620" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
+    <workbookView xWindow="100" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Components" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,14 +19,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="116">
   <si>
     <t>Component</t>
   </si>
   <si>
-    <t>architecture</t>
-  </si>
-  <si>
     <t>schema</t>
   </si>
   <si>
@@ -78,9 +75,6 @@
     <t>d1_instance_generator</t>
   </si>
   <si>
-    <t>PEM</t>
-  </si>
-  <si>
     <t>certificates</t>
   </si>
   <si>
@@ -249,18 +243,12 @@
     <t>Base DataONE library in Python</t>
   </si>
   <si>
-    <t xml:space="preserve">          </t>
-  </si>
-  <si>
     <t>The `Metacat application`_. Currently employed as the replicated object  store on Coordinating Nodes.</t>
   </si>
   <si>
     <t>Coordinating node service, implementing the service APIs, data storage, and CN replication.</t>
   </si>
   <si>
-    <t>Indexes metadata and implements search interfaces for discovery of content stored in the DataONE network. Implemented using Mercury_, as an extension of SOLR_, which in turn is an extension of Lucene_.</t>
-  </si>
-  <si>
     <t>Manages the synchronization of content between Member Nodes and the Coordinating Nodes.</t>
   </si>
   <si>
@@ -295,6 +283,90 @@
   </si>
   <si>
     <t>Debian packages for the CN components</t>
+  </si>
+  <si>
+    <t>d1_architecture</t>
+  </si>
+  <si>
+    <t>A HTTP echo service used for testing</t>
+  </si>
+  <si>
+    <t>x509</t>
+  </si>
+  <si>
+    <t>hzpeek</t>
+  </si>
+  <si>
+    <t>A tool for examining the Hazelcast queues on the CNs</t>
+  </si>
+  <si>
+    <t>A simple search interface using Javascript and the SOLR interface.</t>
+  </si>
+  <si>
+    <t>Operations documentation - servers etc</t>
+  </si>
+  <si>
+    <t>Member node integration testing service</t>
+  </si>
+  <si>
+    <t>Integration testing for components and combinations thereof</t>
+  </si>
+  <si>
+    <t>Generation and management of certificates for use by server components</t>
+  </si>
+  <si>
+    <t>Generates example instances of objects defined in dataoneTypes.xsd</t>
+  </si>
+  <si>
+    <t>The search interface that is implemented by the Mercury search index</t>
+  </si>
+  <si>
+    <t>Populates the SOLR index by extracting informaton from system metadata, science metadata and resource maps.</t>
+  </si>
+  <si>
+    <t>Generates indexing tasks when new objects appear or system metadata changes</t>
+  </si>
+  <si>
+    <t>Code shared between the indexing components</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A library used by the index_processor for extracting content from various types of XML structures such as system metadata, science metadata and resource maps. </t>
+  </si>
+  <si>
+    <t>A library of code shared between coordintating node components</t>
+  </si>
+  <si>
+    <t>A member node implementation and instance for the Dryad repository</t>
+  </si>
+  <si>
+    <t>Mercury implementation of the Member Node services</t>
+  </si>
+  <si>
+    <t>An extention of the FUSE driver that is based on Dokan_ for use on Microsoft Windows systems.</t>
+  </si>
+  <si>
+    <t>Implements the certificate manager used by the portal servlets</t>
+  </si>
+  <si>
+    <t>Provides a UI for interacting with the CILogon service, an authentication proxy service</t>
+  </si>
+  <si>
+    <t>Provides mechanisms for managing subjects in dataone</t>
+  </si>
+  <si>
+    <t>A register of coordinating and member nodes participating in a DataONE environment</t>
+  </si>
+  <si>
+    <t>Manages replication of content between Member Nodes</t>
+  </si>
+  <si>
+    <t>Monitors content on member nodes, creating tasks for synchronization and replication</t>
+  </si>
+  <si>
+    <t>The coordinating node HTTP REST service interface</t>
+  </si>
+  <si>
+    <t>Proxies requests coming in to a CN to underlying service implementations such as the object store (i.e. Metacat)</t>
   </si>
 </sst>
 </file>
@@ -343,8 +415,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="35">
+  <cellStyleXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -386,7 +462,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="35">
+  <cellStyles count="39">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -404,6 +480,8 @@
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -421,6 +499,8 @@
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -750,10 +830,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -768,736 +848,822 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="E1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="G1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>88</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E4" t="s">
-        <v>60</v>
+        <v>58</v>
+      </c>
+      <c r="G4" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E6" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G6" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="G7" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="E8" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G8" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E9" t="s">
-        <v>63</v>
+        <v>61</v>
+      </c>
+      <c r="G9" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B10" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10" t="s">
         <v>12</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E10" t="s">
-        <v>63</v>
+        <v>58</v>
+      </c>
+      <c r="G10" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B11" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="D11" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E11" t="s">
         <v>61</v>
       </c>
+      <c r="G11" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B12" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
+        <v>90</v>
       </c>
       <c r="D12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E12" t="s">
-        <v>60</v>
+        <v>59</v>
+      </c>
+      <c r="G12" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D13" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E13" t="s">
-        <v>62</v>
+        <v>60</v>
+      </c>
+      <c r="G13" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E14" t="s">
-        <v>64</v>
+        <v>62</v>
+      </c>
+      <c r="G14" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B15" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C15" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E15" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G15" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B16" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C16" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D16" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E16" t="s">
-        <v>65</v>
+        <v>63</v>
+      </c>
+      <c r="G16" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="17" spans="1:7">
       <c r="A17" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B17" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C17" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D17" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G17" t="s">
-        <v>76</v>
+        <v>101</v>
       </c>
     </row>
     <row r="18" spans="1:7">
       <c r="A18" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B18" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C18" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D18" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E18" t="s">
-        <v>65</v>
+        <v>63</v>
+      </c>
+      <c r="G18" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="19" spans="1:7">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C19" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D19" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E19" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G19" t="s">
-        <v>79</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="1:7">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B20" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D20" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E20" t="s">
-        <v>67</v>
+        <v>65</v>
+      </c>
+      <c r="G20" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="21" spans="1:7">
       <c r="A21" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B21" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C21" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E21" t="s">
-        <v>67</v>
+        <v>65</v>
+      </c>
+      <c r="G21" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="22" spans="1:7">
       <c r="A22" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B22" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C22" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D22" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E22" t="s">
-        <v>67</v>
+        <v>65</v>
+      </c>
+      <c r="G22" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="23" spans="1:7">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C23" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D23" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E23" t="s">
-        <v>61</v>
+        <v>59</v>
+      </c>
+      <c r="G23" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="24" spans="1:7">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B24" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D24" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E24" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G24" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="25" spans="1:7">
       <c r="A25" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C25" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D25" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E25" t="s">
-        <v>66</v>
+        <v>64</v>
+      </c>
+      <c r="G25" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="26" spans="1:7">
       <c r="A26" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B26" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C26" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D26" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E26" t="s">
-        <v>61</v>
+        <v>59</v>
+      </c>
+      <c r="G26" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="27" spans="1:7">
       <c r="A27" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B27" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C27" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D27" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E27" t="s">
-        <v>61</v>
+        <v>59</v>
+      </c>
+      <c r="G27" t="s">
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:7">
       <c r="A28" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B28" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C28" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D28" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E28" t="s">
-        <v>61</v>
+        <v>59</v>
+      </c>
+      <c r="G28" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="29" spans="1:7">
       <c r="A29" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B29" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C29" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D29" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E29" t="s">
-        <v>61</v>
+        <v>59</v>
+      </c>
+      <c r="G29" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="30" spans="1:7">
       <c r="A30" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B30" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C30" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D30" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E30" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G30" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:7">
       <c r="A31" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B31" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C31" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D31" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E31" t="s">
-        <v>60</v>
+        <v>58</v>
+      </c>
+      <c r="G31" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="32" spans="1:7">
       <c r="A32" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B32" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C32" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D32" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E32" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G32" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="33" spans="1:7">
       <c r="A33" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B33" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C33" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D33" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E33" t="s">
-        <v>68</v>
+        <v>66</v>
+      </c>
+      <c r="G33" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="34" spans="1:7">
       <c r="A34" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B34" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C34" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D34" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E34" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G34" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="35" spans="1:7">
       <c r="A35" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B35" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C35" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D35" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E35" t="s">
-        <v>69</v>
+        <v>67</v>
+      </c>
+      <c r="G35" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="36" spans="1:7">
       <c r="A36" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B36" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C36" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D36" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E36" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="G36" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="37" spans="1:7">
       <c r="A37" t="s">
+        <v>47</v>
+      </c>
+      <c r="B37" t="s">
+        <v>4</v>
+      </c>
+      <c r="C37" t="s">
+        <v>12</v>
+      </c>
+      <c r="D37" t="s">
         <v>49</v>
       </c>
-      <c r="B37" t="s">
-        <v>5</v>
-      </c>
-      <c r="C37" t="s">
-        <v>13</v>
-      </c>
-      <c r="D37" t="s">
-        <v>51</v>
-      </c>
       <c r="E37" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G37" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="38" spans="1:7">
       <c r="A38" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B38" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C38" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D38" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E38" t="s">
-        <v>60</v>
+        <v>58</v>
+      </c>
+      <c r="G38" t="s">
+        <v>107</v>
       </c>
     </row>
     <row r="39" spans="1:7">
       <c r="A39" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B39" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C39" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D39" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E39" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="G39" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B40" t="s">
-        <v>89</v>
+        <v>4</v>
       </c>
       <c r="C40" t="s">
-        <v>90</v>
+        <v>11</v>
       </c>
       <c r="D40" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E40" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G40" t="s">
-        <v>91</v>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" t="s">
+        <v>84</v>
+      </c>
+      <c r="B41" t="s">
+        <v>85</v>
+      </c>
+      <c r="C41" t="s">
+        <v>86</v>
+      </c>
+      <c r="D41" t="s">
+        <v>44</v>
+      </c>
+      <c r="E41" t="s">
+        <v>59</v>
+      </c>
+      <c r="G41" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated REST urls for setObsoletedBy and deleteReplicationMetadta
</commit_message>
<xml_diff>
--- a/source/implementation/data/components.xlsx
+++ b/source/implementation/data/components.xlsx
@@ -18,8 +18,48 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Dave Vieglais</author>
+  </authors>
+  <commentList>
+    <comment ref="F1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Dave Vieglais:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Approximate version 1.0 release implementation status on a scale of 0 (conceptual only) through 4 (complete and immutable)
+0 = concept
+1 = prrof of concept implementation
+2 = production implementation in progress
+3 = production implementation being tested
+4 = production ready or released
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="125">
   <si>
     <t>Component</t>
   </si>
@@ -192,9 +232,6 @@
     <t>MJ</t>
   </si>
   <si>
-    <t>BS</t>
-  </si>
-  <si>
     <t>DV</t>
   </si>
   <si>
@@ -225,9 +262,6 @@
     <t>JG</t>
   </si>
   <si>
-    <t>Status</t>
-  </si>
-  <si>
     <t>Description</t>
   </si>
   <si>
@@ -273,9 +307,6 @@
     <t>A plugin for R that enables access to DataONE content from the R_ application. Implemented using d1_libclient_java.</t>
   </si>
   <si>
-    <t>debian_packaing</t>
-  </si>
-  <si>
     <t>installer</t>
   </si>
   <si>
@@ -367,13 +398,49 @@
   </si>
   <si>
     <t>Proxies requests coming in to a CN to underlying service implementations such as the object store (i.e. Metacat)</t>
+  </si>
+  <si>
+    <t>Tagged as version 1.0.0</t>
+  </si>
+  <si>
+    <t>Stable, but still many sections in draft form or that need  updating.</t>
+  </si>
+  <si>
+    <t>Needs refactoring ot better integration installation notes and other operational information</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Need to document the certificates required and the process for generating and managing them - for both testing and operations</t>
+  </si>
+  <si>
+    <t>Needs to be updated with stable schema</t>
+  </si>
+  <si>
+    <t>Verification pending index availability</t>
+  </si>
+  <si>
+    <t>Pending alterations to lock behavior</t>
+  </si>
+  <si>
+    <t>Status_v1</t>
+  </si>
+  <si>
+    <t>No UI</t>
+  </si>
+  <si>
+    <t>Needs to be updated to be inline with recent index schema changes</t>
+  </si>
+  <si>
+    <t>debian_packaging</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -397,6 +464,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -415,8 +495,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="39">
+  <cellStyleXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -462,7 +544,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="39">
+  <cellStyles count="41">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -482,6 +564,7 @@
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -501,6 +584,7 @@
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -829,21 +913,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G41"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="21.83203125" customWidth="1"/>
     <col min="2" max="2" width="21.6640625" customWidth="1"/>
-    <col min="7" max="7" width="75.83203125" customWidth="1"/>
+    <col min="7" max="7" width="45" style="1" customWidth="1"/>
+    <col min="8" max="8" width="75.83203125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -860,13 +948,16 @@
         <v>55</v>
       </c>
       <c r="F1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+        <v>121</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
         <v>52</v>
       </c>
@@ -882,13 +973,19 @@
       <c r="E2" t="s">
         <v>56</v>
       </c>
+      <c r="F2">
+        <v>4</v>
+      </c>
       <c r="G2" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>113</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="30">
       <c r="A3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -902,11 +999,17 @@
       <c r="E3" t="s">
         <v>57</v>
       </c>
-      <c r="G3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+      <c r="F3">
+        <v>3</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="30">
       <c r="A4" t="s">
         <v>53</v>
       </c>
@@ -920,13 +1023,19 @@
         <v>54</v>
       </c>
       <c r="E4" t="s">
-        <v>58</v>
-      </c>
-      <c r="G4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>57</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -940,13 +1049,16 @@
         <v>42</v>
       </c>
       <c r="E5" t="s">
-        <v>59</v>
-      </c>
-      <c r="G5" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>58</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -960,13 +1072,16 @@
         <v>42</v>
       </c>
       <c r="E6" t="s">
-        <v>60</v>
-      </c>
-      <c r="G6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+        <v>59</v>
+      </c>
+      <c r="F6">
+        <v>3</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -980,13 +1095,16 @@
         <v>42</v>
       </c>
       <c r="E7" t="s">
-        <v>61</v>
-      </c>
-      <c r="G7" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>60</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1000,13 +1118,16 @@
         <v>42</v>
       </c>
       <c r="E8" t="s">
-        <v>60</v>
-      </c>
-      <c r="G8" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>59</v>
+      </c>
+      <c r="F8">
+        <v>3</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1020,13 +1141,16 @@
         <v>43</v>
       </c>
       <c r="E9" t="s">
-        <v>61</v>
-      </c>
-      <c r="G9" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>60</v>
+      </c>
+      <c r="F9">
+        <v>3</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -1040,13 +1164,16 @@
         <v>43</v>
       </c>
       <c r="E10" t="s">
-        <v>58</v>
-      </c>
-      <c r="G10" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>57</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1060,13 +1187,16 @@
         <v>43</v>
       </c>
       <c r="E11" t="s">
-        <v>61</v>
-      </c>
-      <c r="G11" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <v>60</v>
+      </c>
+      <c r="F11">
+        <v>3</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="45">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1074,19 +1204,25 @@
         <v>18</v>
       </c>
       <c r="C12" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="D12" t="s">
         <v>43</v>
       </c>
       <c r="E12" t="s">
-        <v>59</v>
-      </c>
-      <c r="G12" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7">
+        <v>58</v>
+      </c>
+      <c r="F12">
+        <v>2</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -1100,13 +1236,19 @@
         <v>43</v>
       </c>
       <c r="E13" t="s">
-        <v>60</v>
-      </c>
-      <c r="G13" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7">
+        <v>59</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
       <c r="A14" t="s">
         <v>19</v>
       </c>
@@ -1120,13 +1262,19 @@
         <v>44</v>
       </c>
       <c r="E14" t="s">
-        <v>62</v>
-      </c>
-      <c r="G14" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7">
+        <v>61</v>
+      </c>
+      <c r="F14">
+        <v>3</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="30">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -1140,13 +1288,16 @@
         <v>44</v>
       </c>
       <c r="E15" t="s">
-        <v>64</v>
-      </c>
-      <c r="G15" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7">
+        <v>63</v>
+      </c>
+      <c r="F15">
+        <v>3</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="30">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -1160,13 +1311,16 @@
         <v>44</v>
       </c>
       <c r="E16" t="s">
-        <v>63</v>
-      </c>
-      <c r="G16" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7">
+        <v>62</v>
+      </c>
+      <c r="F16">
+        <v>2</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
       <c r="A17" t="s">
         <v>22</v>
       </c>
@@ -1180,13 +1334,16 @@
         <v>44</v>
       </c>
       <c r="E17" t="s">
-        <v>63</v>
-      </c>
-      <c r="G17" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7">
+        <v>62</v>
+      </c>
+      <c r="F17">
+        <v>2</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
       <c r="A18" t="s">
         <v>23</v>
       </c>
@@ -1200,13 +1357,16 @@
         <v>44</v>
       </c>
       <c r="E18" t="s">
-        <v>63</v>
-      </c>
-      <c r="G18" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7">
+        <v>62</v>
+      </c>
+      <c r="F18">
+        <v>2</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="30">
       <c r="A19" t="s">
         <v>24</v>
       </c>
@@ -1220,13 +1380,16 @@
         <v>44</v>
       </c>
       <c r="E19" t="s">
-        <v>63</v>
-      </c>
-      <c r="G19" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7">
+        <v>62</v>
+      </c>
+      <c r="F19">
+        <v>2</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -1240,13 +1403,16 @@
         <v>44</v>
       </c>
       <c r="E20" t="s">
-        <v>65</v>
-      </c>
-      <c r="G20" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
+        <v>64</v>
+      </c>
+      <c r="F20">
+        <v>2</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8">
       <c r="A21" t="s">
         <v>26</v>
       </c>
@@ -1260,13 +1426,16 @@
         <v>44</v>
       </c>
       <c r="E21" t="s">
-        <v>65</v>
-      </c>
-      <c r="G21" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7">
+        <v>64</v>
+      </c>
+      <c r="F21">
+        <v>2</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
       <c r="A22" t="s">
         <v>27</v>
       </c>
@@ -1280,13 +1449,16 @@
         <v>44</v>
       </c>
       <c r="E22" t="s">
-        <v>65</v>
-      </c>
-      <c r="G22" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7">
+        <v>64</v>
+      </c>
+      <c r="F22">
+        <v>2</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
       <c r="A23" t="s">
         <v>28</v>
       </c>
@@ -1300,13 +1472,19 @@
         <v>44</v>
       </c>
       <c r="E23" t="s">
-        <v>59</v>
-      </c>
-      <c r="G23" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7">
+        <v>58</v>
+      </c>
+      <c r="F23">
+        <v>3</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" ht="30">
       <c r="A24" t="s">
         <v>29</v>
       </c>
@@ -1320,13 +1498,16 @@
         <v>44</v>
       </c>
       <c r="E24" t="s">
-        <v>59</v>
-      </c>
-      <c r="G24" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7">
+        <v>58</v>
+      </c>
+      <c r="F24">
+        <v>3</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
       <c r="A25" t="s">
         <v>30</v>
       </c>
@@ -1340,13 +1521,19 @@
         <v>44</v>
       </c>
       <c r="E25" t="s">
-        <v>64</v>
-      </c>
-      <c r="G25" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7">
+        <v>63</v>
+      </c>
+      <c r="F25">
+        <v>3</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8">
       <c r="A26" t="s">
         <v>31</v>
       </c>
@@ -1360,13 +1547,19 @@
         <v>44</v>
       </c>
       <c r="E26" t="s">
-        <v>59</v>
-      </c>
-      <c r="G26" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7">
+        <v>58</v>
+      </c>
+      <c r="F26">
+        <v>3</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
       <c r="A27" t="s">
         <v>32</v>
       </c>
@@ -1380,13 +1573,16 @@
         <v>44</v>
       </c>
       <c r="E27" t="s">
-        <v>59</v>
-      </c>
-      <c r="G27" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7">
+        <v>58</v>
+      </c>
+      <c r="F27">
+        <v>3</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8">
       <c r="A28" t="s">
         <v>33</v>
       </c>
@@ -1400,13 +1596,16 @@
         <v>44</v>
       </c>
       <c r="E28" t="s">
-        <v>59</v>
-      </c>
-      <c r="G28" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7">
+        <v>58</v>
+      </c>
+      <c r="F28">
+        <v>3</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" ht="30">
       <c r="A29" t="s">
         <v>34</v>
       </c>
@@ -1420,13 +1619,16 @@
         <v>44</v>
       </c>
       <c r="E29" t="s">
-        <v>59</v>
-      </c>
-      <c r="G29" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7">
+        <v>58</v>
+      </c>
+      <c r="F29">
+        <v>3</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
       <c r="A30" t="s">
         <v>35</v>
       </c>
@@ -1440,13 +1642,16 @@
         <v>44</v>
       </c>
       <c r="E30" t="s">
-        <v>59</v>
-      </c>
-      <c r="G30" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7">
+        <v>58</v>
+      </c>
+      <c r="F30">
+        <v>3</v>
+      </c>
+      <c r="H30" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" ht="30">
       <c r="A31" t="s">
         <v>36</v>
       </c>
@@ -1460,13 +1665,19 @@
         <v>44</v>
       </c>
       <c r="E31" t="s">
-        <v>58</v>
-      </c>
-      <c r="G31" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7">
+        <v>57</v>
+      </c>
+      <c r="F31">
+        <v>2</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
       <c r="A32" t="s">
         <v>37</v>
       </c>
@@ -1480,13 +1691,16 @@
         <v>45</v>
       </c>
       <c r="E32" t="s">
-        <v>64</v>
-      </c>
-      <c r="G32" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7">
+        <v>63</v>
+      </c>
+      <c r="F32">
+        <v>3</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8">
       <c r="A33" t="s">
         <v>38</v>
       </c>
@@ -1500,13 +1714,16 @@
         <v>45</v>
       </c>
       <c r="E33" t="s">
-        <v>66</v>
-      </c>
-      <c r="G33" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7">
+        <v>65</v>
+      </c>
+      <c r="F33">
+        <v>2</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" ht="30">
       <c r="A34" t="s">
         <v>39</v>
       </c>
@@ -1520,13 +1737,16 @@
         <v>45</v>
       </c>
       <c r="E34" t="s">
-        <v>60</v>
-      </c>
-      <c r="G34" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7">
+        <v>59</v>
+      </c>
+      <c r="F34">
+        <v>3</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8">
       <c r="A35" t="s">
         <v>40</v>
       </c>
@@ -1540,13 +1760,16 @@
         <v>45</v>
       </c>
       <c r="E35" t="s">
-        <v>67</v>
-      </c>
-      <c r="G35" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7">
+        <v>66</v>
+      </c>
+      <c r="F35">
+        <v>3</v>
+      </c>
+      <c r="H35" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" ht="30">
       <c r="A36" t="s">
         <v>46</v>
       </c>
@@ -1560,13 +1783,16 @@
         <v>49</v>
       </c>
       <c r="E36" t="s">
-        <v>60</v>
-      </c>
-      <c r="G36" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7">
+        <v>59</v>
+      </c>
+      <c r="F36">
+        <v>3</v>
+      </c>
+      <c r="H36" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
       <c r="A37" t="s">
         <v>47</v>
       </c>
@@ -1580,13 +1806,16 @@
         <v>49</v>
       </c>
       <c r="E37" t="s">
-        <v>58</v>
-      </c>
-      <c r="G37" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7">
+        <v>57</v>
+      </c>
+      <c r="F37">
+        <v>1</v>
+      </c>
+      <c r="H37" s="1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" ht="30">
       <c r="A38" t="s">
         <v>50</v>
       </c>
@@ -1600,13 +1829,16 @@
         <v>49</v>
       </c>
       <c r="E38" t="s">
-        <v>58</v>
-      </c>
-      <c r="G38" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7">
+        <v>57</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+      <c r="H38" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" ht="30">
       <c r="A39" t="s">
         <v>48</v>
       </c>
@@ -1622,13 +1854,16 @@
       <c r="E39" t="s">
         <v>56</v>
       </c>
-      <c r="G39" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7">
+      <c r="F39">
+        <v>1</v>
+      </c>
+      <c r="H39" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8">
       <c r="A40" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B40" t="s">
         <v>4</v>
@@ -1640,35 +1875,42 @@
         <v>43</v>
       </c>
       <c r="E40" t="s">
-        <v>58</v>
-      </c>
-      <c r="G40" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7">
+        <v>57</v>
+      </c>
+      <c r="F40">
+        <v>2</v>
+      </c>
+      <c r="H40" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
       <c r="A41" t="s">
-        <v>84</v>
+        <v>124</v>
       </c>
       <c r="B41" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C41" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D41" t="s">
         <v>44</v>
       </c>
       <c r="E41" t="s">
-        <v>59</v>
-      </c>
-      <c r="G41" t="s">
-        <v>87</v>
+        <v>58</v>
+      </c>
+      <c r="F41">
+        <v>3</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>